<commit_message>
update chart to 28feb and lyx
</commit_message>
<xml_diff>
--- a/2.4.xlsx
+++ b/2.4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13480" windowHeight="8390" activeTab="1" xr2:uid="{37FAFD38-5033-4608-9D5E-D1AF76AE8584}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13480" windowHeight="8390" activeTab="2" xr2:uid="{37FAFD38-5033-4608-9D5E-D1AF76AE8584}"/>
   </bookViews>
   <sheets>
     <sheet name="ETH" sheetId="1" r:id="rId1"/>
@@ -225,10 +225,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$B$2:$B$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$B$2:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>43009</c:v>
                 </c:pt>
@@ -672,16 +672,25 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$G$2:$G$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$G$2:$G$1529</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="1528"/>
                 <c:pt idx="0">
                   <c:v>15197500</c:v>
                 </c:pt>
@@ -1125,6 +1134,15 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>3518296.387718075</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>3520039.1291030878</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>3521781.8714880967</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>3523524.6148731061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1152,10 +1170,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$B$2:$B$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$B$2:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>43009</c:v>
                 </c:pt>
@@ -1599,16 +1617,25 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$J$2:$J$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$J$2:$J$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>15197500</c:v>
                 </c:pt>
@@ -2052,6 +2079,15 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>4903995.3085201625</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>5176289.260500785</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>5214240.8961708816</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>5011234.6982138529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2096,10 +2132,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$C$2:$C$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$C$2:$C$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>303.95</c:v>
                 </c:pt>
@@ -2543,6 +2579,15 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>840.28</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>867.62</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>871.58</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>851.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2616,7 +2661,7 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="15"/>
+        <c:majorUnit val="16"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
@@ -2934,10 +2979,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$B$2:$B$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$B$2:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>43009</c:v>
                 </c:pt>
@@ -3381,16 +3426,25 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$H$2:$H$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$H$2:$H$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3834,6 +3888,15 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>1.4077936352650051</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1.4859608390401102</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1.4968552109109743</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1.4385776888991193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3865,10 +3928,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$B$2:$B$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$B$2:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>43009</c:v>
                 </c:pt>
@@ -4312,16 +4375,25 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$E$2:$E$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$E$2:$E$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4765,6 +4837,15 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1.0105</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1.0109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1.0115000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4812,10 +4893,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$C$2:$C$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$C$2:$C$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>303.95</c:v>
                 </c:pt>
@@ -5259,6 +5340,15 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>840.28</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>867.62</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>871.58</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>851.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5332,7 +5422,7 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="15"/>
+        <c:majorUnit val="16"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
@@ -8674,10 +8764,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$B$100:$B$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$B$100:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>43107</c:v>
                 </c:pt>
@@ -8827,16 +8917,25 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$G$100:$G$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$G$100:$G$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>15197500</c:v>
                 </c:pt>
@@ -8986,6 +9085,15 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>3518296.387718075</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3520039.1291030878</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3521781.8714880967</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3523524.6148731061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9013,10 +9121,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$B$100:$B$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$B$100:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>43107</c:v>
                 </c:pt>
@@ -9166,16 +9274,25 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$J$100:$J$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$J$100:$J$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>15197500</c:v>
                 </c:pt>
@@ -9325,6 +9442,15 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>4903995.3085201625</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5176289.260500785</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5214240.8961708816</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5011234.6982138529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9354,10 +9480,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$B$100:$B$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$B$100:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>43107</c:v>
                 </c:pt>
@@ -9507,16 +9633,25 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$L$100:$L$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$L$100:$L$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -9666,6 +9801,15 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>14427460.573947404</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>14896883.590194037</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>14964876.097302184</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>14620106.010753812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9869,10 +10013,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 M Case'!$C$100:$C$149</c:f>
+              <c:f>'Oct17-Feb18 M Case'!$C$100:$C$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>1117.75</c:v>
                 </c:pt>
@@ -10022,6 +10166,15 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>840.28</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>867.62</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>871.58</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>851.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13094,10 +13247,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 I Case'!$B$2:$B$149</c:f>
+              <c:f>'Oct17-Feb18 I Case'!$B$2:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>43009</c:v>
                 </c:pt>
@@ -13541,16 +13694,25 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 I Case'!$M$2:$M$149</c:f>
+              <c:f>'Oct17-Feb18 I Case'!$M$2:$M$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -13994,6 +14156,15 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>7.5588310612611176E-2</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>7.612084656450957E-2</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>7.6653382582208218E-2</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>7.7185918665707565E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14038,10 +14209,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 I Case'!$B$2:$B$149</c:f>
+              <c:f>'Oct17-Feb18 I Case'!$B$2:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>43009</c:v>
                 </c:pt>
@@ -14485,16 +14656,25 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 I Case'!$L$2:$L$149</c:f>
+              <c:f>'Oct17-Feb18 I Case'!$L$2:$L$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -14938,6 +15118,15 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>1.7645336404013818</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1.8544826451719034</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1.8675111037999672</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1.8014476065142295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15011,7 +15200,7 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="15"/>
+        <c:majorUnit val="16"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
@@ -15232,10 +15421,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 I Case'!$B$2:$B$149</c:f>
+              <c:f>'Oct17-Feb18 I Case'!$B$2:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>43009</c:v>
                 </c:pt>
@@ -15679,16 +15868,25 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 I Case'!$N$2:$N$149</c:f>
+              <c:f>'Oct17-Feb18 I Case'!$N$2:$N$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -16132,6 +16330,15 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>1.8648951613307494</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2.0239674684571116</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2.0461378861550341</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1.927541762276805</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16176,10 +16383,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Oct17-Feb18 I Case'!$B$2:$B$149</c:f>
+              <c:f>'Oct17-Feb18 I Case'!$B$2:$B$152</c:f>
               <c:numCache>
                 <c:formatCode>yyyy-mm-dd</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>43009</c:v>
                 </c:pt>
@@ -16623,16 +16830,25 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>43156</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43157</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43158</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Oct17-Feb18 I Case'!$L$2:$L$149</c:f>
+              <c:f>'Oct17-Feb18 I Case'!$L$2:$L$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="151"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -17076,6 +17292,15 @@
                 </c:pt>
                 <c:pt idx="147">
                   <c:v>1.7645336404013818</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1.8544826451719034</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1.8675111037999672</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1.8014476065142295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17149,7 +17374,7 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="15"/>
+        <c:majorUnit val="16"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
@@ -22423,8 +22648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B878752-2CAC-455D-9130-AE654B9FB1A1}">
   <dimension ref="A1:B1519"/>
   <sheetViews>
-    <sheetView topLeftCell="A764" workbookViewId="0">
-      <selection activeCell="A788" sqref="A788:B935"/>
+    <sheetView topLeftCell="A890" workbookViewId="0">
+      <selection activeCell="A936" sqref="A936:B938"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29914,13 +30139,28 @@
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A936" s="1"/>
+      <c r="A936" s="1">
+        <v>43157</v>
+      </c>
+      <c r="B936">
+        <v>867.62</v>
+      </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A937" s="1"/>
+      <c r="A937" s="1">
+        <v>43158</v>
+      </c>
+      <c r="B937">
+        <v>871.58</v>
+      </c>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A938" s="1"/>
+      <c r="A938" s="1">
+        <v>43159</v>
+      </c>
+      <c r="B938">
+        <v>851.5</v>
+      </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A939" s="1"/>
@@ -31672,9 +31912,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC12A5B-9A95-44BE-8A49-9BDD3A8403D4}">
-  <dimension ref="A1:X149"/>
+  <dimension ref="A1:X152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="AJ53" sqref="AJ53"/>
     </sheetView>
   </sheetViews>
@@ -38511,6 +38751,141 @@
       </c>
       <c r="Q149" s="1"/>
     </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>21</v>
+      </c>
+      <c r="B150" s="1">
+        <v>43157</v>
+      </c>
+      <c r="C150">
+        <v>867.62</v>
+      </c>
+      <c r="D150">
+        <f t="shared" ref="D150:D152" si="22">C150/$C$129</f>
+        <v>1.2482304195200551</v>
+      </c>
+      <c r="E150">
+        <f t="shared" ref="E150:E152" si="23">1+$U$2*A150</f>
+        <v>1.0105</v>
+      </c>
+      <c r="F150">
+        <v>3483462.7700179</v>
+      </c>
+      <c r="G150">
+        <f t="shared" ref="G150:G152" si="24">E150*F150</f>
+        <v>3520039.1291030878</v>
+      </c>
+      <c r="H150">
+        <f t="shared" ref="H150:H152" si="25">D150*(1+$U$1)-$U$1*E150</f>
+        <v>1.4859608390401102</v>
+      </c>
+      <c r="I150">
+        <v>3483462.7700179</v>
+      </c>
+      <c r="J150">
+        <f t="shared" ref="J150:J152" si="26">H150*I150</f>
+        <v>5176289.260500785</v>
+      </c>
+      <c r="K150">
+        <f t="shared" ref="K150:K152" si="27">J150+G150</f>
+        <v>8696328.3896038719</v>
+      </c>
+      <c r="L150">
+        <f t="shared" ref="L150:L152" si="28">($N$129+$O$129)*C150</f>
+        <v>14896883.590194037</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>22</v>
+      </c>
+      <c r="B151" s="1">
+        <v>43158</v>
+      </c>
+      <c r="C151">
+        <v>871.58</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="22"/>
+        <v>1.2539276054554871</v>
+      </c>
+      <c r="E151">
+        <f t="shared" si="23"/>
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="F151">
+        <v>3483463.7700179</v>
+      </c>
+      <c r="G151">
+        <f t="shared" si="24"/>
+        <v>3521781.8714880967</v>
+      </c>
+      <c r="H151">
+        <f t="shared" si="25"/>
+        <v>1.4968552109109743</v>
+      </c>
+      <c r="I151">
+        <v>3483463.7700179</v>
+      </c>
+      <c r="J151">
+        <f t="shared" si="26"/>
+        <v>5214240.8961708816</v>
+      </c>
+      <c r="K151">
+        <f t="shared" si="27"/>
+        <v>8736022.7676589787</v>
+      </c>
+      <c r="L151">
+        <f t="shared" si="28"/>
+        <v>14964876.097302184</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>23</v>
+      </c>
+      <c r="B152" s="1">
+        <v>43159</v>
+      </c>
+      <c r="C152">
+        <v>851.5</v>
+      </c>
+      <c r="D152">
+        <f t="shared" si="22"/>
+        <v>1.2250388444495597</v>
+      </c>
+      <c r="E152">
+        <f t="shared" si="23"/>
+        <v>1.0115000000000001</v>
+      </c>
+      <c r="F152">
+        <v>3483464.7700179</v>
+      </c>
+      <c r="G152">
+        <f t="shared" si="24"/>
+        <v>3523524.6148731061</v>
+      </c>
+      <c r="H152">
+        <f t="shared" si="25"/>
+        <v>1.4385776888991193</v>
+      </c>
+      <c r="I152">
+        <v>3483464.7700179</v>
+      </c>
+      <c r="J152">
+        <f t="shared" si="26"/>
+        <v>5011234.6982138529</v>
+      </c>
+      <c r="K152">
+        <f t="shared" si="27"/>
+        <v>8534759.3130869586</v>
+      </c>
+      <c r="L152">
+        <f t="shared" si="28"/>
+        <v>14620106.010753812</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -38519,10 +38894,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B1644C-024C-4CF0-A2D1-43BFF4FDEEB2}">
-  <dimension ref="A1:Z149"/>
+  <dimension ref="A1:Z152"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Z33" sqref="Z33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z31" sqref="Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -46825,6 +47200,165 @@
       </c>
       <c r="S149" s="1"/>
     </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>21</v>
+      </c>
+      <c r="B150" s="1">
+        <v>43157</v>
+      </c>
+      <c r="C150">
+        <v>867.62</v>
+      </c>
+      <c r="D150">
+        <f t="shared" ref="D150:D152" si="29">C150/$C$129</f>
+        <v>1.2482304195200551</v>
+      </c>
+      <c r="E150">
+        <f t="shared" ref="E150:E152" si="30">1+$W$2*A150</f>
+        <v>1.0105</v>
+      </c>
+      <c r="F150">
+        <v>16184410.2579556</v>
+      </c>
+      <c r="G150">
+        <f t="shared" ref="G150:G152" si="31">E150*F150</f>
+        <v>16354346.565664133</v>
+      </c>
+      <c r="H150">
+        <f t="shared" ref="H150:H152" si="32">D150*(1+$W$1)-$W$1*E150</f>
+        <v>1.4859608390401102</v>
+      </c>
+      <c r="I150">
+        <v>30927292.560121398</v>
+      </c>
+      <c r="J150">
+        <f t="shared" ref="J150:J152" si="33">H150*I150</f>
+        <v>45956745.601876952</v>
+      </c>
+      <c r="K150">
+        <f t="shared" ref="K150:K152" si="34">J150+G150</f>
+        <v>62311092.167541087</v>
+      </c>
+      <c r="L150">
+        <f t="shared" ref="L150:L152" si="35">C150/$C$2-1</f>
+        <v>1.8544826451719034</v>
+      </c>
+      <c r="M150">
+        <f t="shared" ref="M150:M152" si="36">G150/$G$2-1</f>
+        <v>7.612084656450957E-2</v>
+      </c>
+      <c r="N150">
+        <f t="shared" ref="N150:N152" si="37">J150/$J$2-1</f>
+        <v>2.0239674684571116</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>22</v>
+      </c>
+      <c r="B151" s="1">
+        <v>43158</v>
+      </c>
+      <c r="C151">
+        <v>871.58</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="29"/>
+        <v>1.2539276054554871</v>
+      </c>
+      <c r="E151">
+        <f t="shared" si="30"/>
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="F151">
+        <v>16184411.2579556</v>
+      </c>
+      <c r="G151">
+        <f t="shared" si="31"/>
+        <v>16362439.78179311</v>
+      </c>
+      <c r="H151">
+        <f t="shared" si="32"/>
+        <v>1.4968552109109743</v>
+      </c>
+      <c r="I151">
+        <v>30927293.560121398</v>
+      </c>
+      <c r="J151">
+        <f t="shared" si="33"/>
+        <v>46293680.52484113</v>
+      </c>
+      <c r="K151">
+        <f t="shared" si="34"/>
+        <v>62656120.30663424</v>
+      </c>
+      <c r="L151">
+        <f t="shared" si="35"/>
+        <v>1.8675111037999672</v>
+      </c>
+      <c r="M151">
+        <f t="shared" si="36"/>
+        <v>7.6653382582208218E-2</v>
+      </c>
+      <c r="N151">
+        <f t="shared" si="37"/>
+        <v>2.0461378861550341</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>23</v>
+      </c>
+      <c r="B152" s="1">
+        <v>43159</v>
+      </c>
+      <c r="C152">
+        <v>851.5</v>
+      </c>
+      <c r="D152">
+        <f t="shared" si="29"/>
+        <v>1.2250388444495597</v>
+      </c>
+      <c r="E152">
+        <f t="shared" si="30"/>
+        <v>1.0115000000000001</v>
+      </c>
+      <c r="F152">
+        <v>16184412.2579556</v>
+      </c>
+      <c r="G152">
+        <f t="shared" si="31"/>
+        <v>16370532.998922089</v>
+      </c>
+      <c r="H152">
+        <f t="shared" si="32"/>
+        <v>1.4385776888991193</v>
+      </c>
+      <c r="I152">
+        <v>30927294.560121398</v>
+      </c>
+      <c r="J152">
+        <f t="shared" si="33"/>
+        <v>44491315.932201743</v>
+      </c>
+      <c r="K152">
+        <f t="shared" si="34"/>
+        <v>60861848.93112383</v>
+      </c>
+      <c r="L152">
+        <f t="shared" si="35"/>
+        <v>1.8014476065142295</v>
+      </c>
+      <c r="M152">
+        <f t="shared" si="36"/>
+        <v>7.7185918665707565E-2</v>
+      </c>
+      <c r="N152">
+        <f t="shared" si="37"/>
+        <v>1.927541762276805</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>